<commit_message>
Mejora de matriz de consistencia
</commit_message>
<xml_diff>
--- a/TESIS AVANCES Y DOCUMENTOS RELACIONADOS/Matriz de consistencia JOSÉ ARROYO.xlsx
+++ b/TESIS AVANCES Y DOCUMENTOS RELACIONADOS/Matriz de consistencia JOSÉ ARROYO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Arroyo\Desktop\Tesis Jose Arroyo\tesisESANtemplatelatex\TESIS AVANCES Y DOCUMENTOS RELACIONADOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C474D2-208B-408E-B3D6-DF584EADCE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BD303E-AEEE-4058-8437-1A3D67BA8973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>PROBLEMA</t>
   </si>
@@ -90,6 +90,9 @@
   <si>
     <t>DEPENDIENTE: Consistencia en la detección de retinopatía diabética a través de modelos de deep learning entre diferentes poblaciones.
 INDEPENDIENTE: Variabilidad en la anotación y etiquetado de imágenes de fondo de ojo debido a diferencias entre anotadores.</t>
+  </si>
+  <si>
+    <t>INDICADORES Y SUS FORMULAS</t>
   </si>
 </sst>
 </file>
@@ -160,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -175,6 +178,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,6 +195,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3909392</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1502474</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C03E334-07D4-6B17-E155-A22183EFED44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17311480" y="1059345"/>
+          <a:ext cx="3776042" cy="1445325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>42497</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>113567</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4472609</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1122535</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA5E260F-FC64-1F34-8797-1372EDFD247D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17220627" y="2623197"/>
+          <a:ext cx="4430112" cy="1008968"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>50651</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>73269</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4306957</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1209261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A1F4F40-BDC9-E3ED-EB21-73D54A188B4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17228781" y="3767312"/>
+          <a:ext cx="4256306" cy="1135992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57980</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4422914</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>989628</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DDDE8BB-FD36-BACF-A7B6-9914B722E7EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17236110" y="4986131"/>
+          <a:ext cx="4364934" cy="939932"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,10 +579,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -406,9 +592,10 @@
     <col min="3" max="3" width="47.42578125" customWidth="1"/>
     <col min="4" max="4" width="62.5703125" customWidth="1"/>
     <col min="5" max="5" width="61.140625" customWidth="1"/>
+    <col min="6" max="6" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -417,7 +604,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -431,8 +618,11 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -448,8 +638,9 @@
       <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -465,8 +656,9 @@
       <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -480,8 +672,9 @@
       <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -495,11 +688,13 @@
       <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="F6" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>